<commit_message>
Arrumado o nome na segunda coluna da planilha de treinamento
</commit_message>
<xml_diff>
--- a/Projeto 2/Drawing Tablet.xlsx
+++ b/Projeto 2/Drawing Tablet.xlsx
@@ -26,7 +26,7 @@
     <t xml:space="preserve">Treinamento</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
+    <t xml:space="preserve">Relevância</t>
   </si>
   <si>
     <t xml:space="preserve">my new drawing tablet came today!! #art #monoprice #newtablet #drawingtablet https://t.co/kmns7igpol</t>
@@ -539,6 +539,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">　</t>
     </r>
@@ -1076,6 +1077,7 @@
         <color rgb="FF000000"/>
         <rFont val="Source Han Sans CN Regular"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">。…… </t>
     </r>
@@ -1632,6 +1634,7 @@
       <color rgb="FF000000"/>
       <name val="Source Han Sans CN Regular"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1727,18 +1730,18 @@
   </sheetPr>
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A285" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B302" activeCellId="0" sqref="B302"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="135.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="11.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="3" style="0" width="8.67"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="14.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>

</xml_diff>